<commit_message>
Search devices test wornking as intended
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/demo.xlsx
+++ b/src/test/resources/xls/demo.xlsx
@@ -9,12 +9,13 @@
     <sheet name="Calculator" sheetId="2" r:id="rId5"/>
     <sheet name="GSMArena-signUp" sheetId="3" r:id="rId6"/>
     <sheet name="Data" sheetId="4" r:id="rId7"/>
+    <sheet name="GSMArena-search" sheetId="5" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="104">
   <si>
     <t>Execute</t>
   </si>
@@ -298,6 +299,66 @@
   </si>
   <si>
     <t>arg9</t>
+  </si>
+  <si>
+    <t>device</t>
+  </si>
+  <si>
+    <t>storage</t>
+  </si>
+  <si>
+    <t>os</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy S20 Ultra 5G</t>
+  </si>
+  <si>
+    <t>128GB/256GB/512GB storage, microSDXC</t>
+  </si>
+  <si>
+    <t>Android 10.0; One UI 2</t>
+  </si>
+  <si>
+    <t>Released 2020, March 6</t>
+  </si>
+  <si>
+    <t>Apple iPhone 7 Plus</t>
+  </si>
+  <si>
+    <t>32GB/128GB/256GB storage, no card slot</t>
+  </si>
+  <si>
+    <t>iOS 10.0.1, up to iOS 13.4</t>
+  </si>
+  <si>
+    <t>Released 2016, September</t>
+  </si>
+  <si>
+    <t>Samsung Galaxy M51</t>
+  </si>
+  <si>
+    <t>64GB/128GB storage, microSDXC</t>
+  </si>
+  <si>
+    <t>Android 10.0; One UI 2.0</t>
+  </si>
+  <si>
+    <t>Not announced yet</t>
+  </si>
+  <si>
+    <t>Apple iPad Pro 11 (2020)</t>
+  </si>
+  <si>
+    <t>128GB/256GB/1TB storage, no card slot</t>
+  </si>
+  <si>
+    <t>iPadOS 13.4</t>
+  </si>
+  <si>
+    <t>Released 2020, March 19</t>
   </si>
 </sst>
 </file>
@@ -373,7 +434,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -486,13 +547,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -567,6 +675,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2449,4 +2590,181 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="1" width="1.67188" style="25" customWidth="1"/>
+    <col min="2" max="2" width="8.85156" style="25" customWidth="1"/>
+    <col min="3" max="3" width="15.3516" style="25" customWidth="1"/>
+    <col min="4" max="4" width="30.8516" style="25" customWidth="1"/>
+    <col min="5" max="5" width="40.8516" style="25" customWidth="1"/>
+    <col min="6" max="6" width="24.3516" style="25" customWidth="1"/>
+    <col min="7" max="7" width="21.8516" style="25" customWidth="1"/>
+    <col min="8" max="256" width="8.85156" style="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="15" customHeight="1">
+      <c r="A1" s="10"/>
+      <c r="B1" t="s" s="2">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="G1" t="s" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2" s="11"/>
+      <c r="B2" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>88</v>
+      </c>
+      <c r="E2" t="s" s="26">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s" s="4">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s" s="4">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="11"/>
+      <c r="B3" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="4">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s" s="4">
+        <v>92</v>
+      </c>
+      <c r="E3" t="s" s="4">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s" s="4">
+        <v>94</v>
+      </c>
+      <c r="G3" t="s" s="4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="11"/>
+      <c r="B4" t="s" s="4">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>96</v>
+      </c>
+      <c r="E4" t="s" s="4">
+        <v>97</v>
+      </c>
+      <c r="F4" t="s" s="4">
+        <v>98</v>
+      </c>
+      <c r="G4" t="s" s="4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" ht="15" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s" s="12">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>51</v>
+      </c>
+      <c r="D5" t="s" s="12">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s" s="12">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s" s="12">
+        <v>102</v>
+      </c>
+      <c r="G5" t="s" s="12">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" s="11"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" ht="15" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" ht="15" customHeight="1">
+      <c r="A8" s="27"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="29"/>
+    </row>
+    <row r="9" ht="15" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="32"/>
+    </row>
+    <row r="10" ht="15" customHeight="1">
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>